<commit_message>
Gear Graphics Update and Attachment stats fix
</commit_message>
<xml_diff>
--- a/stats info.xlsx
+++ b/stats info.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="460" windowWidth="15420" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Player</t>
   </si>
@@ -49,15 +50,44 @@
   <si>
     <t>Equipment</t>
   </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +110,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -364,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A11:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C15" zoomScale="115" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="C15" zoomScale="115" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -870,4 +905,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>89</v>
+      </c>
+      <c r="C2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>106</v>
+      </c>
+      <c r="C3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>126</v>
+      </c>
+      <c r="C4">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>151</v>
+      </c>
+      <c r="C5">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>179</v>
+      </c>
+      <c r="C6">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>213</v>
+      </c>
+      <c r="C7">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>254</v>
+      </c>
+      <c r="C8">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>302</v>
+      </c>
+      <c r="C9">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>359</v>
+      </c>
+      <c r="C10">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>428</v>
+      </c>
+      <c r="C11">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1012</v>
+      </c>
+      <c r="C12">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>2405</v>
+      </c>
+      <c r="C13">
+        <v>14664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>5714</v>
+      </c>
+      <c r="C14">
+        <v>35485</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>13583</v>
+      </c>
+      <c r="C15">
+        <v>84973</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>32299</v>
+      </c>
+      <c r="C16">
+        <v>202635</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>76810</v>
+      </c>
+      <c r="C17">
+        <v>482435</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>182673</v>
+      </c>
+      <c r="C18">
+        <v>1147854</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>434458</v>
+      </c>
+      <c r="C19">
+        <v>2730431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>